<commit_message>
Added stats for Tower of Hanoi
</commit_message>
<xml_diff>
--- a/doc/SortingAlgos.xlsx
+++ b/doc/SortingAlgos.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="897"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="897" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sorting" sheetId="12" r:id="rId1"/>
     <sheet name="Wiki" sheetId="14" r:id="rId2"/>
     <sheet name="Sheet7" sheetId="13" r:id="rId3"/>
     <sheet name="Complexity Graph" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="229">
   <si>
     <t>Notes</t>
   </si>
@@ -1528,13 +1529,32 @@
   <si>
     <t>an efficient algorithm for sorting strings</t>
   </si>
+  <si>
+    <t>Tower of Hanoi</t>
+  </si>
+  <si>
+    <t>Disks</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -1864,7 +1884,7 @@
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1999,51 +2019,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2067,6 +2042,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2095,6 +2079,15 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2104,10 +2097,40 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -10764,7 +10787,7 @@
             <c:numRef>
               <c:f>'Complexity Graph'!$N$102:$N$220</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -14878,25 +14901,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="165059968"/>
-        <c:axId val="197096960"/>
+        <c:axId val="36867456"/>
+        <c:axId val="36885632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165059968"/>
+        <c:axId val="36867456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197096960"/>
+        <c:crossAx val="36885632"/>
         <c:crossesAt val="1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197096960"/>
+        <c:axId val="36885632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14909,7 +14932,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165059968"/>
+        <c:crossAx val="36867456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -14918,12 +14941,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -24324,7 +24348,7 @@
             <c:numRef>
               <c:f>'Complexity Graph'!$N$102:$N$220</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -27688,11 +27712,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125542784"/>
-        <c:axId val="125544320"/>
+        <c:axId val="71363200"/>
+        <c:axId val="71401856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125542784"/>
+        <c:axId val="71363200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27716,14 +27740,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125544320"/>
+        <c:crossAx val="71401856"/>
         <c:crossesAt val="1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125544320"/>
+        <c:axId val="71401856"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -27735,7 +27759,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125542784"/>
+        <c:crossAx val="71363200"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -27750,7 +27774,7 @@
           <c:x val="0.91648539600881662"/>
           <c:y val="0.73753862489268351"/>
           <c:w val="7.84271637794553E-2"/>
-          <c:h val="0.20845740650988601"/>
+          <c:h val="0.20845740650988603"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -27758,7 +27782,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -33320,8 +33344,8 @@
       <xdr:rowOff>130969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -33632,7 +33656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -34062,32 +34086,32 @@
       <c r="C1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53" t="s">
+      <c r="E1" s="81"/>
+      <c r="F1" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="52"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="81"/>
       <c r="M1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="52"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="81"/>
       <c r="R1" s="17" t="s">
         <v>78</v>
       </c>
@@ -34150,15 +34174,15 @@
       <c r="C2" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
       <c r="I2" s="18" t="s">
         <v>106</v>
       </c>
@@ -34172,12 +34196,12 @@
       <c r="M2" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="N2" s="56" t="s">
+      <c r="N2" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="57"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60"/>
       <c r="R2" s="18" t="s">
         <v>104</v>
       </c>
@@ -34240,23 +34264,23 @@
       <c r="C3" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58" t="s">
+      <c r="E3" s="60"/>
+      <c r="F3" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="60"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
       <c r="I3" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="57"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="18" t="s">
         <v>104</v>
       </c>
@@ -34332,10 +34356,10 @@
       <c r="C4" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="12" t="s">
         <v>202</v>
       </c>
@@ -34346,11 +34370,11 @@
       <c r="I4" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="J4" s="62" t="s">
+      <c r="J4" s="76" t="s">
         <v>201</v>
       </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="64"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="78"/>
       <c r="M4" s="18" t="s">
         <v>104</v>
       </c>
@@ -34430,28 +34454,28 @@
       <c r="E5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="58">
         <v>1</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="57"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
       <c r="I5" s="18">
         <v>1</v>
       </c>
-      <c r="J5" s="82" t="s">
+      <c r="J5" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="K5" s="83"/>
-      <c r="L5" s="84"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
       <c r="M5" s="18">
         <v>1</v>
       </c>
-      <c r="N5" s="56">
+      <c r="N5" s="58">
         <v>1</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="57"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="22" t="s">
         <v>106</v>
       </c>
@@ -34514,32 +34538,32 @@
       <c r="C6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="76" t="s">
+      <c r="E6" s="65"/>
+      <c r="F6" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="78"/>
-      <c r="H6" s="77"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="74"/>
-      <c r="L6" s="75"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="63"/>
       <c r="M6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="79" t="s">
+      <c r="N6" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="81"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="69"/>
       <c r="R6" s="23" t="s">
         <v>47</v>
       </c>
@@ -34602,32 +34626,32 @@
       <c r="C7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="58" t="s">
+      <c r="E7" s="72"/>
+      <c r="F7" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="72"/>
       <c r="I7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="58" t="s">
+      <c r="J7" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="72"/>
       <c r="M7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="58" t="s">
+      <c r="N7" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="60"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="72"/>
       <c r="R7" s="20" t="s">
         <v>59</v>
       </c>
@@ -34690,30 +34714,30 @@
       <c r="C8" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70" t="s">
+      <c r="E8" s="54"/>
+      <c r="F8" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
       <c r="I8" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="41"/>
-      <c r="N8" s="65" t="s">
+      <c r="N8" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="67"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="52"/>
       <c r="R8" s="42" t="s">
         <v>79</v>
       </c>
@@ -34760,6 +34784,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:H8"/>
@@ -34775,18 +34811,6 @@
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" r:id="rId1" tooltip="Quicksort" display="https://en.wikipedia.org/wiki/Quicksort"/>
@@ -35461,8 +35485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A99:R220"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N223" sqref="N223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35477,7 +35501,7 @@
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="1" customWidth="1"/>
     <col min="15" max="17" width="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -35594,7 +35618,7 @@
         <f>A102 * A102</f>
         <v>0</v>
       </c>
-      <c r="N102" s="1">
+      <c r="N102">
         <f>A102 * A102 * A102</f>
         <v>0</v>
       </c>
@@ -35666,7 +35690,7 @@
         <f>A103 * A103</f>
         <v>1</v>
       </c>
-      <c r="N103" s="1">
+      <c r="N103">
         <f>A103 * A103 * A103</f>
         <v>1</v>
       </c>
@@ -35738,7 +35762,7 @@
         <f t="shared" ref="M104:M167" si="9">A104 * A104</f>
         <v>4</v>
       </c>
-      <c r="N104" s="1">
+      <c r="N104">
         <f t="shared" ref="N104:N167" si="10">A104 * A104 * A104</f>
         <v>8</v>
       </c>
@@ -35810,7 +35834,7 @@
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="N105" s="1">
+      <c r="N105">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
@@ -35882,7 +35906,7 @@
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="N106" s="1">
+      <c r="N106">
         <f t="shared" si="10"/>
         <v>64</v>
       </c>
@@ -35954,7 +35978,7 @@
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="N107" s="1">
+      <c r="N107">
         <f t="shared" si="10"/>
         <v>125</v>
       </c>
@@ -36026,7 +36050,7 @@
         <f t="shared" si="9"/>
         <v>36</v>
       </c>
-      <c r="N108" s="1">
+      <c r="N108">
         <f t="shared" si="10"/>
         <v>216</v>
       </c>
@@ -36098,7 +36122,7 @@
         <f t="shared" si="9"/>
         <v>49</v>
       </c>
-      <c r="N109" s="1">
+      <c r="N109">
         <f t="shared" si="10"/>
         <v>343</v>
       </c>
@@ -36170,7 +36194,7 @@
         <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="N110" s="1">
+      <c r="N110">
         <f t="shared" si="10"/>
         <v>512</v>
       </c>
@@ -36242,7 +36266,7 @@
         <f t="shared" si="9"/>
         <v>81</v>
       </c>
-      <c r="N111" s="1">
+      <c r="N111">
         <f t="shared" si="10"/>
         <v>729</v>
       </c>
@@ -36314,7 +36338,7 @@
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="N112" s="1">
+      <c r="N112">
         <f t="shared" si="10"/>
         <v>1000</v>
       </c>
@@ -36386,7 +36410,7 @@
         <f t="shared" si="9"/>
         <v>121</v>
       </c>
-      <c r="N113" s="1">
+      <c r="N113">
         <f t="shared" si="10"/>
         <v>1331</v>
       </c>
@@ -36458,7 +36482,7 @@
         <f t="shared" si="9"/>
         <v>144</v>
       </c>
-      <c r="N114" s="1">
+      <c r="N114">
         <f t="shared" si="10"/>
         <v>1728</v>
       </c>
@@ -36530,7 +36554,7 @@
         <f t="shared" si="9"/>
         <v>169</v>
       </c>
-      <c r="N115" s="1">
+      <c r="N115">
         <f t="shared" si="10"/>
         <v>2197</v>
       </c>
@@ -36602,7 +36626,7 @@
         <f t="shared" si="9"/>
         <v>196</v>
       </c>
-      <c r="N116" s="1">
+      <c r="N116">
         <f t="shared" si="10"/>
         <v>2744</v>
       </c>
@@ -36674,7 +36698,7 @@
         <f t="shared" si="9"/>
         <v>225</v>
       </c>
-      <c r="N117" s="1">
+      <c r="N117">
         <f t="shared" si="10"/>
         <v>3375</v>
       </c>
@@ -36746,7 +36770,7 @@
         <f t="shared" si="9"/>
         <v>256</v>
       </c>
-      <c r="N118" s="1">
+      <c r="N118">
         <f t="shared" si="10"/>
         <v>4096</v>
       </c>
@@ -36818,7 +36842,7 @@
         <f t="shared" si="9"/>
         <v>289</v>
       </c>
-      <c r="N119" s="1">
+      <c r="N119">
         <f t="shared" si="10"/>
         <v>4913</v>
       </c>
@@ -36890,7 +36914,7 @@
         <f t="shared" si="9"/>
         <v>324</v>
       </c>
-      <c r="N120" s="1">
+      <c r="N120">
         <f t="shared" si="10"/>
         <v>5832</v>
       </c>
@@ -36962,7 +36986,7 @@
         <f t="shared" si="9"/>
         <v>361</v>
       </c>
-      <c r="N121" s="1">
+      <c r="N121">
         <f t="shared" si="10"/>
         <v>6859</v>
       </c>
@@ -37034,7 +37058,7 @@
         <f t="shared" si="9"/>
         <v>400</v>
       </c>
-      <c r="N122" s="1">
+      <c r="N122">
         <f t="shared" si="10"/>
         <v>8000</v>
       </c>
@@ -37106,7 +37130,7 @@
         <f t="shared" si="9"/>
         <v>441</v>
       </c>
-      <c r="N123" s="1">
+      <c r="N123">
         <f t="shared" si="10"/>
         <v>9261</v>
       </c>
@@ -37178,7 +37202,7 @@
         <f t="shared" si="9"/>
         <v>484</v>
       </c>
-      <c r="N124" s="1">
+      <c r="N124">
         <f t="shared" si="10"/>
         <v>10648</v>
       </c>
@@ -37250,7 +37274,7 @@
         <f t="shared" si="9"/>
         <v>529</v>
       </c>
-      <c r="N125" s="1">
+      <c r="N125">
         <f t="shared" si="10"/>
         <v>12167</v>
       </c>
@@ -37322,7 +37346,7 @@
         <f t="shared" si="9"/>
         <v>576</v>
       </c>
-      <c r="N126" s="1">
+      <c r="N126">
         <f t="shared" si="10"/>
         <v>13824</v>
       </c>
@@ -37394,7 +37418,7 @@
         <f t="shared" si="9"/>
         <v>625</v>
       </c>
-      <c r="N127" s="1">
+      <c r="N127">
         <f t="shared" si="10"/>
         <v>15625</v>
       </c>
@@ -37466,7 +37490,7 @@
         <f t="shared" si="9"/>
         <v>676</v>
       </c>
-      <c r="N128" s="1">
+      <c r="N128">
         <f t="shared" si="10"/>
         <v>17576</v>
       </c>
@@ -37538,7 +37562,7 @@
         <f t="shared" si="9"/>
         <v>729</v>
       </c>
-      <c r="N129" s="1">
+      <c r="N129">
         <f t="shared" si="10"/>
         <v>19683</v>
       </c>
@@ -37610,7 +37634,7 @@
         <f t="shared" si="9"/>
         <v>784</v>
       </c>
-      <c r="N130" s="1">
+      <c r="N130">
         <f t="shared" si="10"/>
         <v>21952</v>
       </c>
@@ -37682,7 +37706,7 @@
         <f t="shared" si="9"/>
         <v>841</v>
       </c>
-      <c r="N131" s="1">
+      <c r="N131">
         <f t="shared" si="10"/>
         <v>24389</v>
       </c>
@@ -37754,7 +37778,7 @@
         <f t="shared" si="9"/>
         <v>900</v>
       </c>
-      <c r="N132" s="1">
+      <c r="N132">
         <f t="shared" si="10"/>
         <v>27000</v>
       </c>
@@ -37826,7 +37850,7 @@
         <f t="shared" si="9"/>
         <v>961</v>
       </c>
-      <c r="N133" s="1">
+      <c r="N133">
         <f t="shared" si="10"/>
         <v>29791</v>
       </c>
@@ -37898,7 +37922,7 @@
         <f t="shared" si="9"/>
         <v>1024</v>
       </c>
-      <c r="N134" s="1">
+      <c r="N134">
         <f t="shared" si="10"/>
         <v>32768</v>
       </c>
@@ -37970,7 +37994,7 @@
         <f t="shared" si="9"/>
         <v>1089</v>
       </c>
-      <c r="N135" s="1">
+      <c r="N135">
         <f t="shared" si="10"/>
         <v>35937</v>
       </c>
@@ -38042,7 +38066,7 @@
         <f t="shared" si="9"/>
         <v>1156</v>
       </c>
-      <c r="N136" s="1">
+      <c r="N136">
         <f t="shared" si="10"/>
         <v>39304</v>
       </c>
@@ -38114,7 +38138,7 @@
         <f t="shared" si="9"/>
         <v>1225</v>
       </c>
-      <c r="N137" s="1">
+      <c r="N137">
         <f t="shared" si="10"/>
         <v>42875</v>
       </c>
@@ -38186,7 +38210,7 @@
         <f t="shared" si="9"/>
         <v>1296</v>
       </c>
-      <c r="N138" s="1">
+      <c r="N138">
         <f t="shared" si="10"/>
         <v>46656</v>
       </c>
@@ -38258,7 +38282,7 @@
         <f t="shared" si="9"/>
         <v>1369</v>
       </c>
-      <c r="N139" s="1">
+      <c r="N139">
         <f t="shared" si="10"/>
         <v>50653</v>
       </c>
@@ -38330,7 +38354,7 @@
         <f t="shared" si="9"/>
         <v>1444</v>
       </c>
-      <c r="N140" s="1">
+      <c r="N140">
         <f t="shared" si="10"/>
         <v>54872</v>
       </c>
@@ -38402,7 +38426,7 @@
         <f t="shared" si="9"/>
         <v>1521</v>
       </c>
-      <c r="N141" s="1">
+      <c r="N141">
         <f t="shared" si="10"/>
         <v>59319</v>
       </c>
@@ -38474,7 +38498,7 @@
         <f t="shared" si="9"/>
         <v>1600</v>
       </c>
-      <c r="N142" s="1">
+      <c r="N142">
         <f t="shared" si="10"/>
         <v>64000</v>
       </c>
@@ -38546,7 +38570,7 @@
         <f t="shared" si="9"/>
         <v>1681</v>
       </c>
-      <c r="N143" s="1">
+      <c r="N143">
         <f t="shared" si="10"/>
         <v>68921</v>
       </c>
@@ -38618,7 +38642,7 @@
         <f t="shared" si="9"/>
         <v>1764</v>
       </c>
-      <c r="N144" s="1">
+      <c r="N144">
         <f t="shared" si="10"/>
         <v>74088</v>
       </c>
@@ -38690,7 +38714,7 @@
         <f t="shared" si="9"/>
         <v>1849</v>
       </c>
-      <c r="N145" s="1">
+      <c r="N145">
         <f t="shared" si="10"/>
         <v>79507</v>
       </c>
@@ -38762,7 +38786,7 @@
         <f t="shared" si="9"/>
         <v>1936</v>
       </c>
-      <c r="N146" s="1">
+      <c r="N146">
         <f t="shared" si="10"/>
         <v>85184</v>
       </c>
@@ -38834,7 +38858,7 @@
         <f t="shared" si="9"/>
         <v>2025</v>
       </c>
-      <c r="N147" s="1">
+      <c r="N147">
         <f t="shared" si="10"/>
         <v>91125</v>
       </c>
@@ -38906,7 +38930,7 @@
         <f t="shared" si="9"/>
         <v>2116</v>
       </c>
-      <c r="N148" s="1">
+      <c r="N148">
         <f t="shared" si="10"/>
         <v>97336</v>
       </c>
@@ -38978,7 +39002,7 @@
         <f t="shared" si="9"/>
         <v>2209</v>
       </c>
-      <c r="N149" s="1">
+      <c r="N149">
         <f t="shared" si="10"/>
         <v>103823</v>
       </c>
@@ -39050,7 +39074,7 @@
         <f t="shared" si="9"/>
         <v>2304</v>
       </c>
-      <c r="N150" s="1">
+      <c r="N150">
         <f t="shared" si="10"/>
         <v>110592</v>
       </c>
@@ -39122,7 +39146,7 @@
         <f t="shared" si="9"/>
         <v>2401</v>
       </c>
-      <c r="N151" s="1">
+      <c r="N151">
         <f t="shared" si="10"/>
         <v>117649</v>
       </c>
@@ -39194,7 +39218,7 @@
         <f t="shared" si="9"/>
         <v>2500</v>
       </c>
-      <c r="N152" s="1">
+      <c r="N152">
         <f t="shared" si="10"/>
         <v>125000</v>
       </c>
@@ -39266,7 +39290,7 @@
         <f t="shared" si="9"/>
         <v>3600</v>
       </c>
-      <c r="N153" s="1">
+      <c r="N153">
         <f t="shared" si="10"/>
         <v>216000</v>
       </c>
@@ -39338,7 +39362,7 @@
         <f t="shared" si="9"/>
         <v>4900</v>
       </c>
-      <c r="N154" s="1">
+      <c r="N154">
         <f t="shared" si="10"/>
         <v>343000</v>
       </c>
@@ -39410,7 +39434,7 @@
         <f t="shared" si="9"/>
         <v>6400</v>
       </c>
-      <c r="N155" s="1">
+      <c r="N155">
         <f t="shared" si="10"/>
         <v>512000</v>
       </c>
@@ -39482,7 +39506,7 @@
         <f t="shared" si="9"/>
         <v>8100</v>
       </c>
-      <c r="N156" s="1">
+      <c r="N156">
         <f t="shared" si="10"/>
         <v>729000</v>
       </c>
@@ -39554,7 +39578,7 @@
         <f t="shared" si="9"/>
         <v>10000</v>
       </c>
-      <c r="N157" s="1">
+      <c r="N157">
         <f t="shared" si="10"/>
         <v>1000000</v>
       </c>
@@ -39626,7 +39650,7 @@
         <f t="shared" si="9"/>
         <v>40000</v>
       </c>
-      <c r="N158" s="1">
+      <c r="N158">
         <f t="shared" si="10"/>
         <v>8000000</v>
       </c>
@@ -39698,7 +39722,7 @@
         <f t="shared" si="9"/>
         <v>90000</v>
       </c>
-      <c r="N159" s="1">
+      <c r="N159">
         <f t="shared" si="10"/>
         <v>27000000</v>
       </c>
@@ -39770,7 +39794,7 @@
         <f t="shared" si="9"/>
         <v>160000</v>
       </c>
-      <c r="N160" s="1">
+      <c r="N160">
         <f t="shared" si="10"/>
         <v>64000000</v>
       </c>
@@ -39842,7 +39866,7 @@
         <f t="shared" si="9"/>
         <v>250000</v>
       </c>
-      <c r="N161" s="1">
+      <c r="N161">
         <f t="shared" si="10"/>
         <v>125000000</v>
       </c>
@@ -39914,7 +39938,7 @@
         <f t="shared" si="9"/>
         <v>360000</v>
       </c>
-      <c r="N162" s="1">
+      <c r="N162">
         <f t="shared" si="10"/>
         <v>216000000</v>
       </c>
@@ -39986,7 +40010,7 @@
         <f t="shared" si="9"/>
         <v>490000</v>
       </c>
-      <c r="N163" s="1">
+      <c r="N163">
         <f t="shared" si="10"/>
         <v>343000000</v>
       </c>
@@ -40058,7 +40082,7 @@
         <f t="shared" si="9"/>
         <v>640000</v>
       </c>
-      <c r="N164" s="1">
+      <c r="N164">
         <f t="shared" si="10"/>
         <v>512000000</v>
       </c>
@@ -40130,7 +40154,7 @@
         <f t="shared" si="9"/>
         <v>810000</v>
       </c>
-      <c r="N165" s="1">
+      <c r="N165">
         <f t="shared" si="10"/>
         <v>729000000</v>
       </c>
@@ -40202,7 +40226,7 @@
         <f t="shared" si="9"/>
         <v>1000000</v>
       </c>
-      <c r="N166" s="1">
+      <c r="N166">
         <f t="shared" si="10"/>
         <v>1000000000</v>
       </c>
@@ -40274,7 +40298,7 @@
         <f t="shared" si="9"/>
         <v>4000000</v>
       </c>
-      <c r="N167" s="1">
+      <c r="N167">
         <f t="shared" si="10"/>
         <v>8000000000</v>
       </c>
@@ -40346,7 +40370,7 @@
         <f t="shared" ref="M168:M220" si="28">A168 * A168</f>
         <v>9000000</v>
       </c>
-      <c r="N168" s="1">
+      <c r="N168">
         <f t="shared" ref="N168:N220" si="29">A168 * A168 * A168</f>
         <v>27000000000</v>
       </c>
@@ -40418,7 +40442,7 @@
         <f t="shared" si="28"/>
         <v>16000000</v>
       </c>
-      <c r="N169" s="1">
+      <c r="N169">
         <f t="shared" si="29"/>
         <v>64000000000</v>
       </c>
@@ -40490,7 +40514,7 @@
         <f t="shared" si="28"/>
         <v>25000000</v>
       </c>
-      <c r="N170" s="1">
+      <c r="N170">
         <f t="shared" si="29"/>
         <v>125000000000</v>
       </c>
@@ -40562,7 +40586,7 @@
         <f t="shared" si="28"/>
         <v>36000000</v>
       </c>
-      <c r="N171" s="1">
+      <c r="N171">
         <f t="shared" si="29"/>
         <v>216000000000</v>
       </c>
@@ -40634,7 +40658,7 @@
         <f t="shared" si="28"/>
         <v>49000000</v>
       </c>
-      <c r="N172" s="1">
+      <c r="N172">
         <f t="shared" si="29"/>
         <v>343000000000</v>
       </c>
@@ -40706,7 +40730,7 @@
         <f t="shared" si="28"/>
         <v>64000000</v>
       </c>
-      <c r="N173" s="1">
+      <c r="N173">
         <f t="shared" si="29"/>
         <v>512000000000</v>
       </c>
@@ -40778,7 +40802,7 @@
         <f t="shared" si="28"/>
         <v>81000000</v>
       </c>
-      <c r="N174" s="1">
+      <c r="N174">
         <f t="shared" si="29"/>
         <v>729000000000</v>
       </c>
@@ -40850,7 +40874,7 @@
         <f t="shared" si="28"/>
         <v>100000000</v>
       </c>
-      <c r="N175" s="1">
+      <c r="N175">
         <f t="shared" si="29"/>
         <v>1000000000000</v>
       </c>
@@ -40922,7 +40946,7 @@
         <f t="shared" si="28"/>
         <v>400000000</v>
       </c>
-      <c r="N176" s="1">
+      <c r="N176">
         <f t="shared" si="29"/>
         <v>8000000000000</v>
       </c>
@@ -40994,7 +41018,7 @@
         <f t="shared" si="28"/>
         <v>900000000</v>
       </c>
-      <c r="N177" s="1">
+      <c r="N177">
         <f t="shared" si="29"/>
         <v>27000000000000</v>
       </c>
@@ -41066,7 +41090,7 @@
         <f t="shared" si="28"/>
         <v>1600000000</v>
       </c>
-      <c r="N178" s="1">
+      <c r="N178">
         <f t="shared" si="29"/>
         <v>64000000000000</v>
       </c>
@@ -41138,7 +41162,7 @@
         <f t="shared" si="28"/>
         <v>2500000000</v>
       </c>
-      <c r="N179" s="1">
+      <c r="N179">
         <f t="shared" si="29"/>
         <v>125000000000000</v>
       </c>
@@ -41210,7 +41234,7 @@
         <f t="shared" si="28"/>
         <v>3600000000</v>
       </c>
-      <c r="N180" s="1">
+      <c r="N180">
         <f t="shared" si="29"/>
         <v>216000000000000</v>
       </c>
@@ -41282,7 +41306,7 @@
         <f t="shared" si="28"/>
         <v>4900000000</v>
       </c>
-      <c r="N181" s="1">
+      <c r="N181">
         <f t="shared" si="29"/>
         <v>343000000000000</v>
       </c>
@@ -41354,7 +41378,7 @@
         <f t="shared" si="28"/>
         <v>6400000000</v>
       </c>
-      <c r="N182" s="1">
+      <c r="N182">
         <f t="shared" si="29"/>
         <v>512000000000000</v>
       </c>
@@ -41426,7 +41450,7 @@
         <f t="shared" si="28"/>
         <v>8100000000</v>
       </c>
-      <c r="N183" s="1">
+      <c r="N183">
         <f t="shared" si="29"/>
         <v>729000000000000</v>
       </c>
@@ -41498,7 +41522,7 @@
         <f t="shared" si="28"/>
         <v>10000000000</v>
       </c>
-      <c r="N184" s="1">
+      <c r="N184">
         <f t="shared" si="29"/>
         <v>1000000000000000</v>
       </c>
@@ -41570,7 +41594,7 @@
         <f t="shared" si="28"/>
         <v>40000000000</v>
       </c>
-      <c r="N185" s="1">
+      <c r="N185">
         <f t="shared" si="29"/>
         <v>8000000000000000</v>
       </c>
@@ -41642,7 +41666,7 @@
         <f t="shared" si="28"/>
         <v>90000000000</v>
       </c>
-      <c r="N186" s="1">
+      <c r="N186">
         <f t="shared" si="29"/>
         <v>2.7E+16</v>
       </c>
@@ -41714,7 +41738,7 @@
         <f t="shared" si="28"/>
         <v>160000000000</v>
       </c>
-      <c r="N187" s="1">
+      <c r="N187">
         <f t="shared" si="29"/>
         <v>6.4E+16</v>
       </c>
@@ -41786,7 +41810,7 @@
         <f t="shared" si="28"/>
         <v>250000000000</v>
       </c>
-      <c r="N188" s="1">
+      <c r="N188">
         <f t="shared" si="29"/>
         <v>1.25E+17</v>
       </c>
@@ -41858,7 +41882,7 @@
         <f t="shared" si="28"/>
         <v>360000000000</v>
       </c>
-      <c r="N189" s="1">
+      <c r="N189">
         <f t="shared" si="29"/>
         <v>2.16E+17</v>
       </c>
@@ -41930,7 +41954,7 @@
         <f t="shared" si="28"/>
         <v>490000000000</v>
       </c>
-      <c r="N190" s="1">
+      <c r="N190">
         <f t="shared" si="29"/>
         <v>3.43E+17</v>
       </c>
@@ -42002,7 +42026,7 @@
         <f t="shared" si="28"/>
         <v>640000000000</v>
       </c>
-      <c r="N191" s="1">
+      <c r="N191">
         <f t="shared" si="29"/>
         <v>5.12E+17</v>
       </c>
@@ -42074,7 +42098,7 @@
         <f t="shared" si="28"/>
         <v>810000000000</v>
       </c>
-      <c r="N192" s="1">
+      <c r="N192">
         <f t="shared" si="29"/>
         <v>7.29E+17</v>
       </c>
@@ -42146,7 +42170,7 @@
         <f t="shared" si="28"/>
         <v>1000000000000</v>
       </c>
-      <c r="N193" s="1">
+      <c r="N193">
         <f t="shared" si="29"/>
         <v>1E+18</v>
       </c>
@@ -42218,7 +42242,7 @@
         <f t="shared" si="28"/>
         <v>4000000000000</v>
       </c>
-      <c r="N194" s="1">
+      <c r="N194">
         <f t="shared" si="29"/>
         <v>8E+18</v>
       </c>
@@ -42290,7 +42314,7 @@
         <f t="shared" si="28"/>
         <v>9000000000000</v>
       </c>
-      <c r="N195" s="1">
+      <c r="N195">
         <f t="shared" si="29"/>
         <v>2.7E+19</v>
       </c>
@@ -42362,7 +42386,7 @@
         <f t="shared" si="28"/>
         <v>16000000000000</v>
       </c>
-      <c r="N196" s="1">
+      <c r="N196">
         <f t="shared" si="29"/>
         <v>6.4E+19</v>
       </c>
@@ -42434,7 +42458,7 @@
         <f t="shared" si="28"/>
         <v>25000000000000</v>
       </c>
-      <c r="N197" s="1">
+      <c r="N197">
         <f t="shared" si="29"/>
         <v>1.25E+20</v>
       </c>
@@ -42506,7 +42530,7 @@
         <f t="shared" si="28"/>
         <v>36000000000000</v>
       </c>
-      <c r="N198" s="1">
+      <c r="N198">
         <f t="shared" si="29"/>
         <v>2.16E+20</v>
       </c>
@@ -42578,7 +42602,7 @@
         <f t="shared" si="28"/>
         <v>49000000000000</v>
       </c>
-      <c r="N199" s="1">
+      <c r="N199">
         <f t="shared" si="29"/>
         <v>3.43E+20</v>
       </c>
@@ -42650,7 +42674,7 @@
         <f t="shared" si="28"/>
         <v>64000000000000</v>
       </c>
-      <c r="N200" s="1">
+      <c r="N200">
         <f t="shared" si="29"/>
         <v>5.12E+20</v>
       </c>
@@ -42722,7 +42746,7 @@
         <f t="shared" si="28"/>
         <v>81000000000000</v>
       </c>
-      <c r="N201" s="1">
+      <c r="N201">
         <f t="shared" si="29"/>
         <v>7.29E+20</v>
       </c>
@@ -42794,7 +42818,7 @@
         <f t="shared" si="28"/>
         <v>100000000000000</v>
       </c>
-      <c r="N202" s="1">
+      <c r="N202">
         <f t="shared" si="29"/>
         <v>1E+21</v>
       </c>
@@ -42866,7 +42890,7 @@
         <f t="shared" si="28"/>
         <v>400000000000000</v>
       </c>
-      <c r="N203" s="1">
+      <c r="N203">
         <f t="shared" si="29"/>
         <v>8E+21</v>
       </c>
@@ -42938,7 +42962,7 @@
         <f t="shared" si="28"/>
         <v>900000000000000</v>
       </c>
-      <c r="N204" s="1">
+      <c r="N204">
         <f t="shared" si="29"/>
         <v>2.7000000000000002E+22</v>
       </c>
@@ -43010,7 +43034,7 @@
         <f t="shared" si="28"/>
         <v>1600000000000000</v>
       </c>
-      <c r="N205" s="1">
+      <c r="N205">
         <f t="shared" si="29"/>
         <v>6.4E+22</v>
       </c>
@@ -43082,7 +43106,7 @@
         <f t="shared" si="28"/>
         <v>2500000000000000</v>
       </c>
-      <c r="N206" s="1">
+      <c r="N206">
         <f t="shared" si="29"/>
         <v>1.25E+23</v>
       </c>
@@ -43154,7 +43178,7 @@
         <f t="shared" si="28"/>
         <v>3600000000000000</v>
       </c>
-      <c r="N207" s="1">
+      <c r="N207">
         <f t="shared" si="29"/>
         <v>2.1600000000000002E+23</v>
       </c>
@@ -43226,7 +43250,7 @@
         <f t="shared" si="28"/>
         <v>4900000000000000</v>
       </c>
-      <c r="N208" s="1">
+      <c r="N208">
         <f t="shared" si="29"/>
         <v>3.4299999999999999E+23</v>
       </c>
@@ -43298,7 +43322,7 @@
         <f t="shared" si="28"/>
         <v>6400000000000000</v>
       </c>
-      <c r="N209" s="1">
+      <c r="N209">
         <f t="shared" si="29"/>
         <v>5.12E+23</v>
       </c>
@@ -43370,7 +43394,7 @@
         <f t="shared" si="28"/>
         <v>8100000000000000</v>
       </c>
-      <c r="N210" s="1">
+      <c r="N210">
         <f t="shared" si="29"/>
         <v>7.2900000000000004E+23</v>
       </c>
@@ -43442,7 +43466,7 @@
         <f t="shared" si="28"/>
         <v>1E+16</v>
       </c>
-      <c r="N211" s="1">
+      <c r="N211">
         <f t="shared" si="29"/>
         <v>9.9999999999999998E+23</v>
       </c>
@@ -43514,7 +43538,7 @@
         <f t="shared" si="28"/>
         <v>4E+16</v>
       </c>
-      <c r="N212" s="1">
+      <c r="N212">
         <f t="shared" si="29"/>
         <v>7.9999999999999999E+24</v>
       </c>
@@ -43586,7 +43610,7 @@
         <f t="shared" si="28"/>
         <v>9E+16</v>
       </c>
-      <c r="N213" s="1">
+      <c r="N213">
         <f t="shared" si="29"/>
         <v>2.7E+25</v>
       </c>
@@ -43658,7 +43682,7 @@
         <f t="shared" si="28"/>
         <v>1.6E+17</v>
       </c>
-      <c r="N214" s="1">
+      <c r="N214">
         <f t="shared" si="29"/>
         <v>6.3999999999999999E+25</v>
       </c>
@@ -43730,7 +43754,7 @@
         <f t="shared" si="28"/>
         <v>2.5E+17</v>
       </c>
-      <c r="N215" s="1">
+      <c r="N215">
         <f t="shared" si="29"/>
         <v>1.25E+26</v>
       </c>
@@ -43802,7 +43826,7 @@
         <f t="shared" si="28"/>
         <v>3.6E+17</v>
       </c>
-      <c r="N216" s="1">
+      <c r="N216">
         <f t="shared" si="29"/>
         <v>2.16E+26</v>
       </c>
@@ -43874,7 +43898,7 @@
         <f t="shared" si="28"/>
         <v>4.9E+17</v>
       </c>
-      <c r="N217" s="1">
+      <c r="N217">
         <f t="shared" si="29"/>
         <v>3.4299999999999999E+26</v>
       </c>
@@ -43946,7 +43970,7 @@
         <f t="shared" si="28"/>
         <v>6.4E+17</v>
       </c>
-      <c r="N218" s="1">
+      <c r="N218">
         <f t="shared" si="29"/>
         <v>5.1199999999999999E+26</v>
       </c>
@@ -44018,7 +44042,7 @@
         <f t="shared" si="28"/>
         <v>8.1E+17</v>
       </c>
-      <c r="N219" s="1">
+      <c r="N219">
         <f t="shared" si="29"/>
         <v>7.2899999999999993E+26</v>
       </c>
@@ -44090,7 +44114,7 @@
         <f t="shared" si="28"/>
         <v>1E+18</v>
       </c>
-      <c r="N220" s="1">
+      <c r="N220">
         <f t="shared" si="29"/>
         <v>1E+27</v>
       </c>
@@ -44116,4 +44140,1414 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D102"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="45.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="87" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="87">
+        <f>POWER(2, A3)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="88">
+        <f>POWER(2, A3)/(24*60*60)</f>
+        <v>2.3148148148148147E-5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="87">
+        <f t="shared" ref="B4:B67" si="0">POWER(2, A4)</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="88">
+        <f t="shared" ref="C4:C26" si="1">POWER(2, A4)/(24*60*60)</f>
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="87">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="88">
+        <f t="shared" si="1"/>
+        <v>9.2592592592592588E-5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="87">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="88">
+        <f t="shared" si="1"/>
+        <v>1.8518518518518518E-4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="87">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="88">
+        <f t="shared" si="1"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="87">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C8" s="88">
+        <f t="shared" si="1"/>
+        <v>7.407407407407407E-4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="87">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="C9" s="88">
+        <f t="shared" si="1"/>
+        <v>1.4814814814814814E-3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="87">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="C10" s="88">
+        <f t="shared" si="1"/>
+        <v>2.9629629629629628E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="87">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="C11" s="88">
+        <f t="shared" si="1"/>
+        <v>5.9259259259259256E-3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="87">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="C12" s="88">
+        <f t="shared" si="1"/>
+        <v>1.1851851851851851E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="87">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="C13" s="88">
+        <f t="shared" si="1"/>
+        <v>2.3703703703703703E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="87">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="C14" s="88">
+        <f t="shared" si="1"/>
+        <v>4.7407407407407405E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="87">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="C15" s="88">
+        <f t="shared" si="1"/>
+        <v>9.481481481481481E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="87">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="C16" s="88">
+        <f t="shared" si="1"/>
+        <v>0.18962962962962962</v>
+      </c>
+      <c r="D16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="87">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="C17" s="88">
+        <f t="shared" si="1"/>
+        <v>0.37925925925925924</v>
+      </c>
+      <c r="D17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="87">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+      <c r="C18" s="88">
+        <f t="shared" si="1"/>
+        <v>0.75851851851851848</v>
+      </c>
+      <c r="D18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="87">
+        <f t="shared" si="0"/>
+        <v>131072</v>
+      </c>
+      <c r="C19" s="88">
+        <f t="shared" si="1"/>
+        <v>1.517037037037037</v>
+      </c>
+      <c r="D19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="87">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="C20" s="88">
+        <f t="shared" si="1"/>
+        <v>3.0340740740740739</v>
+      </c>
+      <c r="D20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="87">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="C21" s="88">
+        <f t="shared" si="1"/>
+        <v>6.0681481481481478</v>
+      </c>
+      <c r="D21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="87">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="C22" s="88">
+        <f t="shared" si="1"/>
+        <v>12.136296296296296</v>
+      </c>
+      <c r="D22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="87">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="C23" s="88">
+        <f t="shared" si="1"/>
+        <v>24.272592592592591</v>
+      </c>
+      <c r="D23" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="87">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="C24" s="88">
+        <f t="shared" si="1"/>
+        <v>48.545185185185183</v>
+      </c>
+      <c r="D24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="87">
+        <f t="shared" si="0"/>
+        <v>8388608</v>
+      </c>
+      <c r="C25" s="88">
+        <f t="shared" si="1"/>
+        <v>97.090370370370366</v>
+      </c>
+      <c r="D25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="87">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+      <c r="C26" s="88">
+        <f t="shared" si="1"/>
+        <v>194.18074074074073</v>
+      </c>
+      <c r="D26" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="87">
+        <f t="shared" si="0"/>
+        <v>33554432</v>
+      </c>
+      <c r="C27" s="88">
+        <f t="shared" ref="C4:C67" si="2">POWER(2, A27)/(356*24*60*60)</f>
+        <v>1.0909030378693301</v>
+      </c>
+      <c r="D27" s="89" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="87">
+        <f t="shared" si="0"/>
+        <v>67108864</v>
+      </c>
+      <c r="C28" s="87">
+        <f t="shared" si="2"/>
+        <v>2.1818060757386601</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="87">
+        <f t="shared" si="0"/>
+        <v>134217728</v>
+      </c>
+      <c r="C29" s="87">
+        <f t="shared" si="2"/>
+        <v>4.3636121514773203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="87">
+        <f t="shared" si="0"/>
+        <v>268435456</v>
+      </c>
+      <c r="C30" s="87">
+        <f t="shared" si="2"/>
+        <v>8.7272243029546406</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="87">
+        <f t="shared" si="0"/>
+        <v>536870912</v>
+      </c>
+      <c r="C31" s="87">
+        <f t="shared" si="2"/>
+        <v>17.454448605909281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="87">
+        <f t="shared" si="0"/>
+        <v>1073741824</v>
+      </c>
+      <c r="C32" s="87">
+        <f t="shared" si="2"/>
+        <v>34.908897211818562</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="87">
+        <f t="shared" si="0"/>
+        <v>2147483648</v>
+      </c>
+      <c r="C33" s="87">
+        <f t="shared" si="2"/>
+        <v>69.817794423637125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="87">
+        <f t="shared" si="0"/>
+        <v>4294967296</v>
+      </c>
+      <c r="C34" s="87">
+        <f t="shared" si="2"/>
+        <v>139.63558884727425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="87">
+        <f t="shared" si="0"/>
+        <v>8589934592</v>
+      </c>
+      <c r="C35" s="87">
+        <f t="shared" si="2"/>
+        <v>279.2711776945485</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="87">
+        <f t="shared" si="0"/>
+        <v>17179869184</v>
+      </c>
+      <c r="C36" s="87">
+        <f t="shared" si="2"/>
+        <v>558.542355389097</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="87">
+        <f t="shared" si="0"/>
+        <v>34359738368</v>
+      </c>
+      <c r="C37" s="87">
+        <f t="shared" si="2"/>
+        <v>1117.084710778194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="87">
+        <f t="shared" si="0"/>
+        <v>68719476736</v>
+      </c>
+      <c r="C38" s="87">
+        <f t="shared" si="2"/>
+        <v>2234.169421556388</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" s="87">
+        <f t="shared" si="0"/>
+        <v>137438953472</v>
+      </c>
+      <c r="C39" s="87">
+        <f t="shared" si="2"/>
+        <v>4468.338843112776</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" s="87">
+        <f t="shared" si="0"/>
+        <v>274877906944</v>
+      </c>
+      <c r="C40" s="87">
+        <f t="shared" si="2"/>
+        <v>8936.677686225552</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" s="87">
+        <f t="shared" si="0"/>
+        <v>549755813888</v>
+      </c>
+      <c r="C41" s="87">
+        <f t="shared" si="2"/>
+        <v>17873.355372451104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" s="87">
+        <f t="shared" si="0"/>
+        <v>1099511627776</v>
+      </c>
+      <c r="C42" s="87">
+        <f t="shared" si="2"/>
+        <v>35746.710744902208</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" s="87">
+        <f t="shared" si="0"/>
+        <v>2199023255552</v>
+      </c>
+      <c r="C43" s="87">
+        <f t="shared" si="2"/>
+        <v>71493.421489804416</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="87">
+        <f t="shared" si="0"/>
+        <v>4398046511104</v>
+      </c>
+      <c r="C44" s="87">
+        <f t="shared" si="2"/>
+        <v>142986.84297960883</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="87">
+        <f t="shared" si="0"/>
+        <v>8796093022208</v>
+      </c>
+      <c r="C45" s="87">
+        <f t="shared" si="2"/>
+        <v>285973.68595921766</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="87">
+        <f t="shared" si="0"/>
+        <v>17592186044416</v>
+      </c>
+      <c r="C46" s="87">
+        <f t="shared" si="2"/>
+        <v>571947.37191843532</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="87">
+        <f t="shared" si="0"/>
+        <v>35184372088832</v>
+      </c>
+      <c r="C47" s="87">
+        <f t="shared" si="2"/>
+        <v>1143894.7438368706</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" s="87">
+        <f t="shared" si="0"/>
+        <v>70368744177664</v>
+      </c>
+      <c r="C48" s="87">
+        <f t="shared" si="2"/>
+        <v>2287789.4876737413</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" s="87">
+        <f t="shared" si="0"/>
+        <v>140737488355328</v>
+      </c>
+      <c r="C49" s="87">
+        <f t="shared" si="2"/>
+        <v>4575578.9753474826</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" s="87">
+        <f t="shared" si="0"/>
+        <v>281474976710656</v>
+      </c>
+      <c r="C50" s="87">
+        <f t="shared" si="2"/>
+        <v>9151157.9506949652</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" s="87">
+        <f t="shared" si="0"/>
+        <v>562949953421312</v>
+      </c>
+      <c r="C51" s="87">
+        <f t="shared" si="2"/>
+        <v>18302315.90138993</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="87">
+        <f t="shared" si="0"/>
+        <v>1125899906842624</v>
+      </c>
+      <c r="C52" s="87">
+        <f t="shared" si="2"/>
+        <v>36604631.802779861</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" s="87">
+        <f t="shared" si="0"/>
+        <v>2251799813685248</v>
+      </c>
+      <c r="C53" s="87">
+        <f t="shared" si="2"/>
+        <v>73209263.605559722</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" s="87">
+        <f t="shared" si="0"/>
+        <v>4503599627370496</v>
+      </c>
+      <c r="C54" s="87">
+        <f t="shared" si="2"/>
+        <v>146418527.21111944</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" s="87">
+        <f t="shared" si="0"/>
+        <v>9007199254740992</v>
+      </c>
+      <c r="C55" s="87">
+        <f t="shared" si="2"/>
+        <v>292837054.42223889</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" s="87">
+        <f t="shared" si="0"/>
+        <v>1.8014398509481984E+16</v>
+      </c>
+      <c r="C56" s="87">
+        <f t="shared" si="2"/>
+        <v>585674108.84447777</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" s="87">
+        <f t="shared" si="0"/>
+        <v>3.6028797018963968E+16</v>
+      </c>
+      <c r="C57" s="87">
+        <f t="shared" si="2"/>
+        <v>1171348217.6889555</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" s="87">
+        <f t="shared" si="0"/>
+        <v>7.2057594037927936E+16</v>
+      </c>
+      <c r="C58" s="87">
+        <f t="shared" si="2"/>
+        <v>2342696435.3779111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" s="87">
+        <f t="shared" si="0"/>
+        <v>1.4411518807585587E+17</v>
+      </c>
+      <c r="C59" s="87">
+        <f t="shared" si="2"/>
+        <v>4685392870.7558222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" s="87">
+        <f t="shared" si="0"/>
+        <v>2.8823037615171174E+17</v>
+      </c>
+      <c r="C60" s="87">
+        <f t="shared" si="2"/>
+        <v>9370785741.5116444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" s="87">
+        <f t="shared" si="0"/>
+        <v>5.7646075230342349E+17</v>
+      </c>
+      <c r="C61" s="87">
+        <f t="shared" si="2"/>
+        <v>18741571483.023289</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" s="87">
+        <f t="shared" si="0"/>
+        <v>1.152921504606847E+18</v>
+      </c>
+      <c r="C62" s="87">
+        <f t="shared" si="2"/>
+        <v>37483142966.046577</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" s="87">
+        <f t="shared" si="0"/>
+        <v>2.305843009213694E+18</v>
+      </c>
+      <c r="C63" s="87">
+        <f t="shared" si="2"/>
+        <v>74966285932.093155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" s="87">
+        <f t="shared" si="0"/>
+        <v>4.6116860184273879E+18</v>
+      </c>
+      <c r="C64" s="87">
+        <f t="shared" si="2"/>
+        <v>149932571864.18631</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" s="87">
+        <f t="shared" si="0"/>
+        <v>9.2233720368547758E+18</v>
+      </c>
+      <c r="C65" s="87">
+        <f t="shared" si="2"/>
+        <v>299865143728.37262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" s="87">
+        <f t="shared" si="0"/>
+        <v>1.8446744073709552E+19</v>
+      </c>
+      <c r="C66" s="87">
+        <f t="shared" si="2"/>
+        <v>599730287456.74524</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" s="87">
+        <f t="shared" si="0"/>
+        <v>3.6893488147419103E+19</v>
+      </c>
+      <c r="C67" s="87">
+        <f t="shared" si="2"/>
+        <v>1199460574913.4905</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" s="87">
+        <f t="shared" ref="B68:B102" si="3">POWER(2, A68)</f>
+        <v>7.3786976294838206E+19</v>
+      </c>
+      <c r="C68" s="87">
+        <f t="shared" ref="C68:C102" si="4">POWER(2, A68)/(356*24*60*60)</f>
+        <v>2398921149826.981</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" s="87">
+        <f t="shared" si="3"/>
+        <v>1.4757395258967641E+20</v>
+      </c>
+      <c r="C69" s="87">
+        <f t="shared" si="4"/>
+        <v>4797842299653.9619</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" s="87">
+        <f t="shared" si="3"/>
+        <v>2.9514790517935283E+20</v>
+      </c>
+      <c r="C70" s="87">
+        <f t="shared" si="4"/>
+        <v>9595684599307.9238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" s="87">
+        <f t="shared" si="3"/>
+        <v>5.9029581035870565E+20</v>
+      </c>
+      <c r="C71" s="87">
+        <f t="shared" si="4"/>
+        <v>19191369198615.848</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" s="87">
+        <f t="shared" si="3"/>
+        <v>1.1805916207174113E+21</v>
+      </c>
+      <c r="C72" s="87">
+        <f t="shared" si="4"/>
+        <v>38382738397231.695</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" s="87">
+        <f t="shared" si="3"/>
+        <v>2.3611832414348226E+21</v>
+      </c>
+      <c r="C73" s="87">
+        <f t="shared" si="4"/>
+        <v>76765476794463.391</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" s="87">
+        <f t="shared" si="3"/>
+        <v>4.7223664828696452E+21</v>
+      </c>
+      <c r="C74" s="87">
+        <f t="shared" si="4"/>
+        <v>153530953588926.78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" s="87">
+        <f t="shared" si="3"/>
+        <v>9.4447329657392904E+21</v>
+      </c>
+      <c r="C75" s="87">
+        <f t="shared" si="4"/>
+        <v>307061907177853.56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" s="87">
+        <f t="shared" si="3"/>
+        <v>1.8889465931478581E+22</v>
+      </c>
+      <c r="C76" s="87">
+        <f t="shared" si="4"/>
+        <v>614123814355707.12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" s="87">
+        <f t="shared" si="3"/>
+        <v>3.7778931862957162E+22</v>
+      </c>
+      <c r="C77" s="87">
+        <f t="shared" si="4"/>
+        <v>1228247628711414.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" s="87">
+        <f t="shared" si="3"/>
+        <v>7.5557863725914323E+22</v>
+      </c>
+      <c r="C78" s="87">
+        <f t="shared" si="4"/>
+        <v>2456495257422828.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" s="87">
+        <f t="shared" si="3"/>
+        <v>1.5111572745182865E+23</v>
+      </c>
+      <c r="C79" s="87">
+        <f t="shared" si="4"/>
+        <v>4912990514845657</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" s="87">
+        <f t="shared" si="3"/>
+        <v>3.0223145490365729E+23</v>
+      </c>
+      <c r="C80" s="87">
+        <f t="shared" si="4"/>
+        <v>9825981029691314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" s="87">
+        <f t="shared" si="3"/>
+        <v>6.0446290980731459E+23</v>
+      </c>
+      <c r="C81" s="87">
+        <f t="shared" si="4"/>
+        <v>1.9651962059382628E+16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" s="87">
+        <f t="shared" si="3"/>
+        <v>1.2089258196146292E+24</v>
+      </c>
+      <c r="C82" s="87">
+        <f t="shared" si="4"/>
+        <v>3.9303924118765256E+16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" s="87">
+        <f t="shared" si="3"/>
+        <v>2.4178516392292583E+24</v>
+      </c>
+      <c r="C83" s="87">
+        <f t="shared" si="4"/>
+        <v>7.8607848237530512E+16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" s="87">
+        <f t="shared" si="3"/>
+        <v>4.8357032784585167E+24</v>
+      </c>
+      <c r="C84" s="87">
+        <f t="shared" si="4"/>
+        <v>1.5721569647506102E+17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" s="87">
+        <f t="shared" si="3"/>
+        <v>9.6714065569170334E+24</v>
+      </c>
+      <c r="C85" s="87">
+        <f t="shared" si="4"/>
+        <v>3.1443139295012205E+17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" s="87">
+        <f t="shared" si="3"/>
+        <v>1.9342813113834067E+25</v>
+      </c>
+      <c r="C86" s="87">
+        <f t="shared" si="4"/>
+        <v>6.288627859002441E+17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" s="87">
+        <f t="shared" si="3"/>
+        <v>3.8685626227668134E+25</v>
+      </c>
+      <c r="C87" s="87">
+        <f t="shared" si="4"/>
+        <v>1.2577255718004882E+18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" s="87">
+        <f t="shared" si="3"/>
+        <v>7.7371252455336267E+25</v>
+      </c>
+      <c r="C88" s="87">
+        <f t="shared" si="4"/>
+        <v>2.5154511436009764E+18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" s="87">
+        <f t="shared" si="3"/>
+        <v>1.5474250491067253E+26</v>
+      </c>
+      <c r="C89" s="87">
+        <f t="shared" si="4"/>
+        <v>5.0309022872019528E+18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" s="87">
+        <f t="shared" si="3"/>
+        <v>3.0948500982134507E+26</v>
+      </c>
+      <c r="C90" s="87">
+        <f t="shared" si="4"/>
+        <v>1.0061804574403906E+19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" s="87">
+        <f t="shared" si="3"/>
+        <v>6.1897001964269014E+26</v>
+      </c>
+      <c r="C91" s="87">
+        <f t="shared" si="4"/>
+        <v>2.0123609148807811E+19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" s="87">
+        <f t="shared" si="3"/>
+        <v>1.2379400392853803E+27</v>
+      </c>
+      <c r="C92" s="87">
+        <f t="shared" si="4"/>
+        <v>4.0247218297615622E+19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" s="87">
+        <f t="shared" si="3"/>
+        <v>2.4758800785707605E+27</v>
+      </c>
+      <c r="C93" s="87">
+        <f t="shared" si="4"/>
+        <v>8.0494436595231244E+19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" s="87">
+        <f t="shared" si="3"/>
+        <v>4.9517601571415211E+27</v>
+      </c>
+      <c r="C94" s="87">
+        <f t="shared" si="4"/>
+        <v>1.6098887319046249E+20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" s="87">
+        <f t="shared" si="3"/>
+        <v>9.9035203142830422E+27</v>
+      </c>
+      <c r="C95" s="87">
+        <f t="shared" si="4"/>
+        <v>3.2197774638092498E+20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" s="87">
+        <f t="shared" si="3"/>
+        <v>1.9807040628566084E+28</v>
+      </c>
+      <c r="C96" s="87">
+        <f t="shared" si="4"/>
+        <v>6.4395549276184995E+20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" s="87">
+        <f t="shared" si="3"/>
+        <v>3.9614081257132169E+28</v>
+      </c>
+      <c r="C97" s="87">
+        <f t="shared" si="4"/>
+        <v>1.2879109855236999E+21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" s="87">
+        <f t="shared" si="3"/>
+        <v>7.9228162514264338E+28</v>
+      </c>
+      <c r="C98" s="87">
+        <f t="shared" si="4"/>
+        <v>2.5758219710473998E+21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" s="87">
+        <f t="shared" si="3"/>
+        <v>1.5845632502852868E+29</v>
+      </c>
+      <c r="C99" s="87">
+        <f t="shared" si="4"/>
+        <v>5.1516439420947996E+21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" s="87">
+        <f t="shared" si="3"/>
+        <v>3.1691265005705735E+29</v>
+      </c>
+      <c r="C100" s="87">
+        <f t="shared" si="4"/>
+        <v>1.0303287884189599E+22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" s="87">
+        <f t="shared" si="3"/>
+        <v>6.338253001141147E+29</v>
+      </c>
+      <c r="C101" s="87">
+        <f t="shared" si="4"/>
+        <v>2.0606575768379199E+22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" s="87">
+        <f t="shared" si="3"/>
+        <v>1.2676506002282294E+30</v>
+      </c>
+      <c r="C102" s="87">
+        <f t="shared" si="4"/>
+        <v>4.1213151536758397E+22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>